<commit_message>
Added pdf of schedule
</commit_message>
<xml_diff>
--- a/Location Details/E Cedar St , Zionsville, IN 46077_arts.xlsx
+++ b/Location Details/E Cedar St , Zionsville, IN 46077_arts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,7 +499,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -520,7 +520,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -541,7 +541,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -604,7 +604,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -625,7 +625,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -634,19 +634,19 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CCA Gallery</t>
+          <t>Carmel Art Education Studio</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="E10" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -655,19 +655,19 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Carmel Art Education Studio</t>
+          <t>Carmel International Arts Festival</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -676,19 +676,19 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Carmel International Arts Festival</t>
+          <t>Cat Head Press: Printshop and Artist Cooperative</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="E12" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -697,40 +697,40 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Cat Head Press: Printshop and Artist Cooperative</t>
+          <t>Clowes Memorial Hall</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="E13" t="n">
-        <v>26</v>
+        <v>797</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CLOSED_TEMPORARILY</t>
+          <t>OPERATIONAL</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CityWay Gallery</t>
+          <t>Corporate Fine Art Group</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3.8</v>
+        <v>5</v>
       </c>
       <c r="E14" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -739,19 +739,19 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Clowes Memorial Hall</t>
+          <t>Creative Energy Arts</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4.7</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>797</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -760,19 +760,19 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Corporate Fine Art Group</t>
+          <t>Creative Expressions Arts</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -781,19 +781,19 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Creative Energy Arts</t>
+          <t>Cultural Arts Gallery</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -802,19 +802,19 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Creative Expressions Arts</t>
+          <t>Dance Arts</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -823,19 +823,19 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Cultural Arts Gallery</t>
+          <t>Dance Magic Performing Arts</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -844,19 +844,19 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dance Arts</t>
+          <t>Edison School Of The Arts</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4.8</v>
+        <v>3.6</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -865,19 +865,19 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dance Magic Performing Arts</t>
+          <t>Gallery 924</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>4.9</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -886,19 +886,19 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Edison School Of The Arts</t>
+          <t>Glass Arts Indiana, Inc.</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.6</v>
+        <v>4.8</v>
       </c>
       <c r="E22" t="n">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -907,19 +907,19 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Gallery 924</t>
+          <t>Harrison Center</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4.9</v>
+        <v>4.8</v>
       </c>
       <c r="E23" t="n">
-        <v>15</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -928,19 +928,19 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Glass Arts Indiana, Inc.</t>
+          <t>Herron School of Art and Design</t>
         </is>
       </c>
       <c r="D24" t="n">
         <v>4.8</v>
       </c>
       <c r="E24" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -949,19 +949,19 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Harrison Center</t>
+          <t>Herron School of Art and Design - Eskenazi Fine Arts Center</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="E25" t="n">
-        <v>134</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -970,19 +970,19 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Herron School of Art and Design</t>
+          <t>High Frequency Arts</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="E26" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -991,19 +991,19 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Herron School of Art and Design - Eskenazi Fine Arts Center</t>
+          <t>Ignition Arts, LLC</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>4.5</v>
+        <v>4.9</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1012,11 +1012,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>High Frequency Arts</t>
+          <t>Indiana Arts Building</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" t="n">
         <v>3</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1033,19 +1033,19 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ignition Arts, LLC</t>
+          <t>Indiana Arts Commission</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1054,19 +1054,19 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Indiana Arts Commission</t>
+          <t>Indiana Fine Arts Academy</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1075,19 +1075,19 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Indiana Fine Arts Academy</t>
+          <t>Indiana Performing Arts Centre</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1096,19 +1096,19 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Indiana Performing Arts Centre</t>
+          <t>Indianapolis Art Center</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1117,19 +1117,19 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Indianapolis Art Center</t>
+          <t>Indianapolis Arts Chorale</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.7</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1138,19 +1138,19 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Indianapolis Arts Chorale</t>
+          <t>Indianapolis Arts Services</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1159,19 +1159,19 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Indianapolis Arts Services</t>
+          <t>Indianapolis Artsgarden</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>5</v>
+        <v>4.6</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1180,19 +1180,19 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Indianapolis Artsgarden</t>
+          <t>Korka International Arts</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>146</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1201,19 +1201,19 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Korka International Arts</t>
+          <t>Landmark Keystone Art Cinema</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>4.4</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>513</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1222,19 +1222,19 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Landmark Keystone Art Cinema</t>
+          <t>Lebanon Community Arts Council-N</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>4.4</v>
+        <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>513</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1271,12 +1271,12 @@
         <v>4.7</v>
       </c>
       <c r="E40" t="n">
-        <v>3894</v>
+        <v>3896</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1360,7 +1360,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1390,19 +1390,19 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Ripple Mobile Arts</t>
+          <t>Schrott Center for the Arts</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1411,19 +1411,19 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Schrott Center for the Arts</t>
+          <t>Sho Arts</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="E47" t="n">
-        <v>106</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Sho Arts</t>
+          <t>Sidney &amp; Lois Eskenazi Fine Arts Center</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1444,7 +1444,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Sidney &amp; Lois Eskenazi Fine Arts Center</t>
+          <t>Steve Haigh Fine Art</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1465,7 +1465,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -1474,19 +1474,19 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Steve Haigh Fine Art</t>
+          <t>Studio Alchemy LLC</t>
         </is>
       </c>
       <c r="D50" t="n">
         <v>5</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -1495,19 +1495,19 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Studio Alchemy LLC</t>
+          <t>The Art Studio of Carmel</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1516,19 +1516,19 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>The Art Studio of Carmel</t>
+          <t>The Carmel Arts Council Children’s Art Gallery</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1537,19 +1537,19 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>The Carmel Arts Council Children’s Art Gallery</t>
+          <t>The Center for the Performing Arts</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -1558,19 +1558,19 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>The Center for the Performing Arts</t>
+          <t>The Murphy Art Center</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>4.7</v>
+        <v>5</v>
       </c>
       <c r="E54" t="n">
-        <v>1193</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -1579,19 +1579,19 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>The Murphy Art Center</t>
+          <t>The Palladium at the Center for the Performing Arts</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>5</v>
+        <v>4.9</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -1600,19 +1600,19 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>The Palladium at the Center for the Performing Arts</t>
+          <t>United Art &amp; Education</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>4.9</v>
+        <v>4.5</v>
       </c>
       <c r="E56" t="n">
-        <v>197</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -1621,19 +1621,19 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>United Art &amp; Education</t>
+          <t>Warren Performing Arts Center</t>
         </is>
       </c>
       <c r="D57" t="n">
         <v>4.5</v>
       </c>
       <c r="E57" t="n">
-        <v>132</v>
+        <v>374</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -1642,19 +1642,19 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Warren Performing Arts Center</t>
+          <t>Zionsville Performing Arts Center</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="E58" t="n">
-        <v>374</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -1663,19 +1663,19 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Zionsville Performing Arts Center</t>
+          <t>carmel academy of the arts</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>4.7</v>
+        <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -1684,34 +1684,13 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>carmel academy of the arts</t>
+          <t>iDREAM Music And Arts Center</t>
         </is>
       </c>
       <c r="D60" t="n">
         <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>OPERATIONAL</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>iDREAM Music And Arts Center</t>
-        </is>
-      </c>
-      <c r="D61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>